<commit_message>
links all relative no absolute links
</commit_message>
<xml_diff>
--- a/example_data/import/project_contents/import 2024-01-25.xlsx
+++ b/example_data/import/project_contents/import 2024-01-25.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/44b92e2d6c7d28b1/Studium/TU Berlin/Masterarbeit/Code/pros/example_data/import/project_contents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonas/Library/Mobile Documents/com~apple~CloudDocs/Coding/python/pros-icloud/example_data/import/project_contents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{0F125187-5C21-A94B-9010-12268AE1388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3B48052-5FED-B845-BE8E-61D8A00E53A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6D54AC-A6F1-DC45-BE5D-18463AD3CE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="51200" windowHeight="26800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,8 +20,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Noch nicht in qgis" guid="{88289622-D034-4E38-A0C0-61CEB0F9C67E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="NKV &lt; 1,5" guid="{23E76F66-981C-4206-9E06-CBB72D7DAC5B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Noch nicht in qgis" guid="{88289622-D034-4E38-A0C0-61CEB0F9C67E}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -483,10 +483,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,9 +688,9 @@
   </sheetPr>
   <dimension ref="A1:BK1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
+      <selection pane="bottomLeft" activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1032,7 +1028,9 @@
       <c r="AW2" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX2" s="15"/>
+      <c r="AX2" s="15">
+        <v>85</v>
+      </c>
       <c r="AY2" s="15" t="b">
         <v>1</v>
       </c>
@@ -1185,7 +1183,9 @@
       <c r="AW3" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX3" s="15"/>
+      <c r="AX3" s="15">
+        <v>78</v>
+      </c>
       <c r="AY3" s="15" t="b">
         <v>1</v>
       </c>
@@ -1340,7 +1340,9 @@
       <c r="AW4" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX4" s="15"/>
+      <c r="AX4" s="15">
+        <v>78</v>
+      </c>
       <c r="AY4" s="15" t="b">
         <v>1</v>
       </c>
@@ -1495,7 +1497,9 @@
       <c r="AW5" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX5" s="15"/>
+      <c r="AX5" s="15">
+        <v>78</v>
+      </c>
       <c r="AY5" s="15" t="b">
         <v>1</v>
       </c>
@@ -1650,7 +1654,9 @@
       <c r="AW6" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX6" s="15"/>
+      <c r="AX6" s="15">
+        <v>78</v>
+      </c>
       <c r="AY6" s="15" t="b">
         <v>1</v>
       </c>
@@ -1805,7 +1811,9 @@
       <c r="AW7" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="AX7" s="15"/>
+      <c r="AX7" s="15">
+        <v>78</v>
+      </c>
       <c r="AY7" s="15" t="b">
         <v>1</v>
       </c>

</xml_diff>